<commit_message>
add UPDATE test conditions for 5 tables
</commit_message>
<xml_diff>
--- a/testdb/updatetestcases/UpdateTestingDocument.xlsx
+++ b/testdb/updatetestcases/UpdateTestingDocument.xlsx
@@ -12,8 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Inital Testing" sheetId="1" r:id="rId1"/>
+    <sheet name=" Intial Testing for CheckUpdate" sheetId="1" r:id="rId1"/>
     <sheet name="Customer" sheetId="2" r:id="rId2"/>
+    <sheet name="Delivery" sheetId="5" r:id="rId3"/>
+    <sheet name="Payment" sheetId="6" r:id="rId4"/>
+    <sheet name="Product" sheetId="3" r:id="rId5"/>
+    <sheet name="Si" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="135">
   <si>
     <t>Test Condition</t>
   </si>
@@ -292,9 +296,6 @@
     <t>updte customer set lname ='roman' ;</t>
   </si>
   <si>
-    <t>update customers set lname = 'roman' ;</t>
-  </si>
-  <si>
     <t>update prodct set lname = 'roman' ;</t>
   </si>
   <si>
@@ -386,6 +387,173 @@
   </si>
   <si>
     <t>update customer last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>UPDATE customer SET birthdate = '3/7/1960' WHERE last_name = 'Ayden' AND email = 'oreneve@wopa.net' ;</t>
+  </si>
+  <si>
+    <t>UPDATE delivery SET quantity = '150',delivery_cost = '10000' WHERE delivery_date = '4/1/2015' ;</t>
+  </si>
+  <si>
+    <t>UPDATE delivery SET quantity = '75',delivery_date = '11/30/2015' WHERE si_id &gt; '1000' AND delivery_cost &gt; '10000' ;</t>
+  </si>
+  <si>
+    <t>UPDATE delivery SET quantity = '75',delivery_date = '11/30/2015' WHERE si_id &gt; '1000' OR delivery_cost &lt; '10000' ;</t>
+  </si>
+  <si>
+    <t>UPDATE payment SET amount = '5500',mode_of_payment = 'debit card' WHERE mode_of_payment = 'none' AND date_of_payment != '5/31/2014' ;</t>
+  </si>
+  <si>
+    <t>UPDATE payment SET amount = '5500',mode_of_payment = 'debit card' WHERE mode_of_payment = 'none' AND date_of_payment != '5/31/2014' OR date_of_payment = '7/14/2014' ;</t>
+  </si>
+  <si>
+    <t>UPDATE product SET description = 'technology' WHERE stock &lt; '87' AND stock &gt; '80' ;</t>
+  </si>
+  <si>
+    <t>UPDATE si SET price = '20000' WHERE customer_id &lt; '4250' AND customer_id &gt; '4000' OR product_id = '3469' ;</t>
+  </si>
+  <si>
+    <t>UPDATE si SET date_ordered = '9/2/2014' WHERE customer_id &lt; '4250' AND customer_id &gt; '4000' AND product_id = '3469' ;</t>
+  </si>
+  <si>
+    <t>UPDATE si SET price = '1999' WHERE product_id &lt; '70' OR product_id = '65' ;</t>
+  </si>
+  <si>
+    <t>UPDATE si SET customer_id = '1001', date_ordered = '10/10/2015' WHERE product_id &lt; '500' AND price &lt; '4000' ;</t>
+  </si>
+  <si>
+    <t>UPDATE si SET product_id = '1111', price = '5850' WHERE customer_id &lt; '1000' ;</t>
+  </si>
+  <si>
+    <t>UPDATE product SET model = '1960s', description = 'imagination' WHERE stock &lt; '30' ;</t>
+  </si>
+  <si>
+    <t>UPDATE product SET description = 'ability' WHERE weight != '0' OR weight &lt; '1' ;</t>
+  </si>
+  <si>
+    <t>UPDATE product SET weight = '25', model = '1980s' WHERE description = 'solution' ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATE payment SET mode_of_payment = 'cash' WHERE mode_of_payment = 'none' ; </t>
+  </si>
+  <si>
+    <t>UPDATE payment SET amount = '4500' WHERE mode_of_payment = 'paypal' AND date_of_payment &lt; '7/30/2014' ;</t>
+  </si>
+  <si>
+    <t>UPDATE payment SET date_of_payment = '6/30/2014',amount = '7500' WHERE mode_of_payment = 'bitcoin' OR mode_of_payment = 'lbc' ;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test Date:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> October 16, 2015</t>
+    </r>
+  </si>
+  <si>
+    <t>UPDATE delivery SET delivery_cost = '1500' WHERE quantity &lt; '10' ;</t>
+  </si>
+  <si>
+    <t>UPDATE delivery SET delivery_cost = '2500', quantity = '50' WHERE si_id &lt; '100' ;</t>
+  </si>
+  <si>
+    <t>UPDATE customer SET last_name = 'Owen',first_name = 'Jerry' WHERE birthdate = '28/3/1928' ;</t>
+  </si>
+  <si>
+    <t>UPDATE customer SET email = 'ay@mail.com' WHERE last_name = 'Ayden' AND birthdate = '7/3/1960' ;</t>
+  </si>
+  <si>
+    <t>UPDATE customer SET first_name = 'George',email = 'george@mail.com' WHERE birthdate = '18/1/1961' AND last_name = 'Henry' ;</t>
+  </si>
+  <si>
+    <t>UPDATE customer SET first_name = 'George' WHERE birthdate = '21/9/2012' OR email = 'zenila@unu.co.uk' ;</t>
+  </si>
+  <si>
+    <t>Query OK, 1 Row(s) affected                                                                        Row(s) matched: 1 Changed: 1</t>
+  </si>
+  <si>
+    <t>Query OK, 27 Row(s) affected                                                                        Row(s) matched: 27 Changed: 27</t>
+  </si>
+  <si>
+    <t>Query OK, 9990 Row(s) affected                                                                        Row(s) matched: 9990 Changed: 9990</t>
+  </si>
+  <si>
+    <t>Query OK, 9993 Row(s) affected                                                                        Row(s) matched: 9993 Changed: 9993</t>
+  </si>
+  <si>
+    <t>Query OK, 37 Row(s) affected                                                                        Row(s) matched: 37 Changed: 37</t>
+  </si>
+  <si>
+    <t>Query OK, 1013 Row(s) affected                                                                        Row(s) matched: 1013 Changed: 1013</t>
+  </si>
+  <si>
+    <t>Query OK, 9957 Row(s) affected                                                                        Row(s) matched: 9957 Changed: 9957</t>
+  </si>
+  <si>
+    <t>Query OK, 1025 Row(s) affected                                                                        Row(s) matched: 1025 Changed: 1025</t>
+  </si>
+  <si>
+    <t>Query OK, 811 Row(s) affected                                                                        Row(s) matched: 811 Changed: 811</t>
+  </si>
+  <si>
+    <t>Query OK, 1891 Row(s) affected                                                                        Row(s) matched: 1891 Changed: 1891</t>
+  </si>
+  <si>
+    <t>Query OK, 633 Row(s) affected                                                                        Row(s) matched: 633 Changed: 633</t>
+  </si>
+  <si>
+    <t>Query OK, 10000 Row(s) affected                                                                        Row(s) matched: 10000 Changed: 10000</t>
+  </si>
+  <si>
+    <t>Query OK, 2409 Row(s) affected                                                                        Row(s) matched: 2409 Changed: 2409</t>
+  </si>
+  <si>
+    <t>Query OK, 799 Row(s) affected                                                                        Row(s) matched: 799 Changed: 799</t>
+  </si>
+  <si>
+    <t>Query OK, 19 Row(s) affected                                                                        Row(s) matched: 19 Changed: 19</t>
+  </si>
+  <si>
+    <t>Query OK, 6713 Row(s) affected                                                                        Row(s) matched: 6713 Changed: 6713</t>
+  </si>
+  <si>
+    <t>Query OK, 6572 Row(s) affected                                                                        Row(s) matched: 6572 Changed: 6572</t>
+  </si>
+  <si>
+    <t>Query OK, 1490 Row(s) affected                                                                        Row(s) matched: 1490 Changed: 1490</t>
+  </si>
+  <si>
+    <t>Query OK, 5 Row(s) affected                                                                        Row(s) matched: 5 Changed: 5</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Check WHERE clause</t>
+  </si>
+  <si>
+    <t>Invalid input 'where clause' does not exist!</t>
+  </si>
+  <si>
+    <t>UPDATE product SET model = '1970s' WHERE  weight &gt; '50' AND stock &gt; '100' ;</t>
+  </si>
+  <si>
+    <t>update customers set lname = 'roman'  ;</t>
   </si>
 </sst>
 </file>
@@ -493,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -553,6 +721,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -843,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,59 +1032,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="28"/>
       <c r="E2" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D9:D98,"PASSED")</f>
-        <v>30</v>
+        <f>COUNTIF(D9:D100,"PASSED")</f>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D9:D98,"FAILED")</f>
+        <f>COUNTIF(D9:D100,"FAILED")</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="25"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D5" s="16">
         <f>SUM(D3:D4)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -964,62 +1137,58 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>4</v>
@@ -1028,13 +1197,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>4</v>
@@ -1043,76 +1212,76 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>5</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="D18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>2</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>4</v>
@@ -1121,13 +1290,13 @@
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>4</v>
@@ -1136,13 +1305,13 @@
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>4</v>
@@ -1151,13 +1320,13 @@
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>4</v>
@@ -1166,13 +1335,13 @@
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>4</v>
@@ -1181,13 +1350,13 @@
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>4</v>
@@ -1196,13 +1365,13 @@
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>4</v>
@@ -1211,13 +1380,13 @@
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>4</v>
@@ -1226,13 +1395,13 @@
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>19</v>
+        <v>67</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>4</v>
@@ -1241,13 +1410,13 @@
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>20</v>
+        <v>68</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>4</v>
@@ -1256,13 +1425,13 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>4</v>
@@ -1271,13 +1440,13 @@
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>4</v>
@@ -1286,13 +1455,13 @@
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>4</v>
@@ -1301,13 +1470,13 @@
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>24</v>
+        <v>72</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>4</v>
@@ -1316,13 +1485,13 @@
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>25</v>
+        <v>73</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>4</v>
@@ -1331,13 +1500,13 @@
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>4</v>
@@ -1346,13 +1515,13 @@
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>4</v>
@@ -1361,13 +1530,13 @@
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>4</v>
@@ -1376,13 +1545,13 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>4</v>
@@ -1391,13 +1560,13 @@
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>4</v>
@@ -1406,13 +1575,13 @@
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>4</v>
@@ -1421,13 +1590,13 @@
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>4</v>
@@ -1436,42 +1605,48 @@
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
+        <v>23</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>24</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>25</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="B45" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>26</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="D45" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
@@ -1480,21 +1655,21 @@
       <c r="D46" s="19"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
-        <v>27</v>
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>26</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1505,14 +1680,24 @@
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="6"/>
+      <c r="A49" s="11">
+        <v>27</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
+      <c r="A50" s="1"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="19"/>
@@ -1526,7 +1711,7 @@
       <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="19"/>
@@ -1650,6 +1835,20 @@
       <c r="C69" s="6"/>
       <c r="D69" s="19"/>
       <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1666,10 +1865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,59 +1881,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="28"/>
       <c r="E2" s="4" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D9:D98,"PASSED")</f>
-        <v>0</v>
+        <f>COUNTIF(D8:D51,"PASSED")</f>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D9:D98,"FAILED")</f>
+        <f>COUNTIF(D8:D53,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="25"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D5" s="16">
         <f>SUM(D3:D4)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1758,441 +1957,170 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="21"/>
+      <c r="B8" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>4</v>
+      </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="19"/>
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>4</v>
+      </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="21"/>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>4</v>
+      </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="19"/>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>4</v>
+      </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="20">
+        <v>6</v>
+      </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>8</v>
+      </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="20">
+        <v>10</v>
+      </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="1">
+        <v>11</v>
+      </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="21"/>
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="20">
+        <v>12</v>
+      </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1">
+        <v>13</v>
+      </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="20">
+        <v>14</v>
+      </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1">
+        <v>15</v>
+      </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="19"/>
       <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="6"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="6"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="6"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="6"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="6"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="6"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="6"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="6"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="6"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="6"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2203,5 +2131,1086 @@
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="E2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14">
+        <f>COUNTIF(D8:D51,"PASSED")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <f>COUNTIF(D8:D53,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="16">
+        <f>SUM(D3:D4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>2</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <v>11</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>13</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>14</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="20">
+        <v>15</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="E2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14">
+        <f>COUNTIF(D8:D51,"PASSED")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <f>COUNTIF(D8:D53,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="16">
+        <f>SUM(D3:D4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>13</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
+        <v>14</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>15</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="E2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14">
+        <f>COUNTIF(D8:D51,"PASSED")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <f>COUNTIF(D8:D53,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="16">
+        <f>SUM(D3:D4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>13</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
+        <v>14</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>15</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="E2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14">
+        <f>COUNTIF(D8:D51,"PASSED")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <f>COUNTIF(D8:D53,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="16">
+        <f>SUM(D3:D4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>2</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>13</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
+        <v>14</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>15</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add test conditions for missing SET/WHERE clause
</commit_message>
<xml_diff>
--- a/testdb/updatetestcases/UpdateTestingDocument.xlsx
+++ b/testdb/updatetestcases/UpdateTestingDocument.xlsx
@@ -1,35 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitscm\CS227Database\testdb\updatetestcases\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name=" Intial Testing for CheckUpdate" sheetId="1" r:id="rId1"/>
+    <sheet name="Check SET_WHERE" sheetId="7" r:id="rId1"/>
     <sheet name="Customer" sheetId="2" r:id="rId2"/>
     <sheet name="Delivery" sheetId="5" r:id="rId3"/>
     <sheet name="Payment" sheetId="6" r:id="rId4"/>
     <sheet name="Product" sheetId="3" r:id="rId5"/>
     <sheet name="Si" sheetId="4" r:id="rId6"/>
+    <sheet name=" Intial Testing for CheckUpdate" sheetId="1" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="175">
   <si>
     <t>Test Condition</t>
   </si>
@@ -176,10 +167,9 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>Component :</t>
     </r>
@@ -199,10 +189,9 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>Analyst:</t>
     </r>
@@ -222,10 +211,9 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>Tester:</t>
     </r>
@@ -245,10 +233,9 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>Developer:</t>
     </r>
@@ -274,10 +261,9 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>Test Date:</t>
     </r>
@@ -447,10 +433,9 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>Test Date:</t>
     </r>
@@ -555,12 +540,151 @@
   <si>
     <t>update customers set lname = 'roman'  ;</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Test Date:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> October 17, 2015</t>
+    </r>
+  </si>
+  <si>
+    <t>update customer set last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>Check table existing/spelling with set/where clause</t>
+  </si>
+  <si>
+    <t>Check column names existing/spelling in each table with set/where clause</t>
+  </si>
+  <si>
+    <t>update prodct set description = 'technology' WHERE stock &lt; '87' AND stock &gt; '80' ;</t>
+  </si>
+  <si>
+    <t>update is set price = '1999' WHERE product_id &lt; '70' OR product_id = '65' ;</t>
+  </si>
+  <si>
+    <t>update delvery set delivery_cost = '2500', quantity = '50' WHERE si_id &lt; '100' ;</t>
+  </si>
+  <si>
+    <t>update pyment set mode_of_payment = 'cash' WHERE mode_of_payment = 'none' ;</t>
+  </si>
+  <si>
+    <t>Check UPDATE spelling</t>
+  </si>
+  <si>
+    <t>Check missing SET</t>
+  </si>
+  <si>
+    <t>Check missing WHERE clause</t>
+  </si>
+  <si>
+    <t>Syntax error in input</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>update customer l_name = 'roman' where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>update customers set l_name = 'roman' where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>update customer set lname = 'roman' where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>update customer set fname = 'ray' where last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>update customer set emails = 'a@gov.com' where last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>update customer set bdate = '7/7/1999' where last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>update customer set cust_id = '8'  where last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>update payment set pay_id = '100' where amount = '5000' ;</t>
+  </si>
+  <si>
+    <t>update payment set sid = '500' where amount = '5000' ;</t>
+  </si>
+  <si>
+    <t>update payment set amt = '5000'  where payment_id = '100' ;</t>
+  </si>
+  <si>
+    <t>update payment set paymentdate = '5/5/2015' where payment_id = '100' ;</t>
+  </si>
+  <si>
+    <t>update payment set paymentmode = 'credit card' where payment_id = '100' ;</t>
+  </si>
+  <si>
+    <t>update si set sid = '1000' where price = '1500' ;</t>
+  </si>
+  <si>
+    <t>update si set cust_id = '1000' where price = '1500' ;</t>
+  </si>
+  <si>
+    <t>update si set prod_id = '1000' where price = '1500' ;</t>
+  </si>
+  <si>
+    <t>update si set dateorder = '10/10/10' where price = '1500' ;</t>
+  </si>
+  <si>
+    <t>update si set prices = '1500' where si_id = '1000' ;</t>
+  </si>
+  <si>
+    <t>update product set p_id = '10' where weight = '350' ;</t>
+  </si>
+  <si>
+    <t>update product set product_model = 'g9xafnhmex' where weight = '350' ;</t>
+  </si>
+  <si>
+    <t>update product set p_stock = '10' where weight = '350' ;</t>
+  </si>
+  <si>
+    <t>update product set p_desc = 'technology' where weight = '350' ;</t>
+  </si>
+  <si>
+    <t>update product set p_weight = '350' where model = '1960s' ;</t>
+  </si>
+  <si>
+    <t>update delivery set d_id = '11111' where delivery_cost = '25000' ;</t>
+  </si>
+  <si>
+    <t>update delivery set sid = '10101' where delivery_cost = '25000' ;</t>
+  </si>
+  <si>
+    <t>update delivery set qty = '15' where delivery_cost = '25000' ;</t>
+  </si>
+  <si>
+    <t>update delivery set date = '11/11/2015' where delivery_cost = '25000' ;</t>
+  </si>
+  <si>
+    <t>update delivery set cost = '25000' where si_id = '10101' ;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,48 +694,47 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -623,13 +746,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor indexed="22"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -727,6 +850,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -742,14 +868,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -796,7 +914,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -831,7 +949,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1008,21 +1126,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -1031,67 +1147,67 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:5" ht="21">
+      <c r="B1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="29"/>
       <c r="E2" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D9:D100,"PASSED")</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+        <f>COUNTIF(D8:D100,"PASSED")</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D9:D100,"FAILED")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+        <f>COUNTIF(D8:D100,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D5" s="16">
         <f>SUM(D3:D4)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -1108,747 +1224,569 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="17"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+    <row r="9" spans="1:5" s="25" customFormat="1">
+      <c r="A9" s="24">
         <v>1</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="17"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="D13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="45">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="45">
+      <c r="A20" s="1">
+        <v>5</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="1">
+        <v>3</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="1">
+        <v>4</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" ht="30">
+      <c r="A27" s="1">
+        <v>5</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="1">
+        <v>6</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="1">
+        <v>7</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="1">
         <v>8</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>2</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>3</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>4</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>5</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="B30" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="30">
+      <c r="A31" s="1">
         <v>9</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>2</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B31" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="30">
+      <c r="A32" s="1">
         <v>10</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>3</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B32" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="30">
+      <c r="A33" s="1">
         <v>11</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>4</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B33" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" ht="30">
+      <c r="A34" s="1">
         <v>12</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>5</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="B34" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" ht="30">
+      <c r="A35" s="1">
         <v>13</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>6</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B35" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" ht="30">
+      <c r="A36" s="1">
         <v>14</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>7</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="B36" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" ht="30">
+      <c r="A37" s="1">
         <v>15</v>
       </c>
-      <c r="D27" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>8</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B37" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" ht="30">
+      <c r="A38" s="1">
         <v>16</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>9</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="B38" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" ht="30">
+      <c r="A39" s="1">
         <v>17</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>10</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="B39" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" ht="30">
+      <c r="A40" s="1">
         <v>18</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>11</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="10" t="s">
+      <c r="B40" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" ht="30">
+      <c r="A41" s="1">
         <v>19</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>12</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="10" t="s">
+      <c r="B41" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" ht="30">
+      <c r="A42" s="1">
         <v>20</v>
       </c>
-      <c r="D32" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>13</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="10" t="s">
+      <c r="B42" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" ht="30">
+      <c r="A43" s="1">
         <v>21</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>14</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="10" t="s">
+      <c r="B43" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" ht="30">
+      <c r="A44" s="1">
         <v>22</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>15</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="10" t="s">
+      <c r="B44" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" ht="30">
+      <c r="A45" s="1">
         <v>23</v>
       </c>
-      <c r="D35" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>16</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="B45" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" ht="30">
+      <c r="A46" s="1">
         <v>24</v>
       </c>
-      <c r="D36" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>17</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="B46" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" ht="30">
+      <c r="A47" s="1">
         <v>25</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>18</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>19</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>20</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>21</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>22</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>23</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>24</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>25</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="B47" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>26</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
-        <v>27</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="6"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="6"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="6"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="6"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="6"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="6"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="6"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="6"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="6"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="6"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="6"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="6"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="6"/>
+      <c r="D47" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1858,20 +1796,22 @@
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -1880,28 +1820,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:5" ht="21">
+      <c r="B1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="29"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1910,11 +1850,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1923,11 +1863,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -1936,11 +1876,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -1957,7 +1897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -1972,7 +1912,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="45">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -1987,7 +1927,7 @@
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -2002,7 +1942,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="60">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -2017,7 +1957,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="45">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -2032,7 +1972,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -2041,7 +1981,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="12" customHeight="1">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2050,7 +1990,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="12" customHeight="1">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -2059,7 +1999,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -2068,7 +2008,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -2077,7 +2017,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -2086,7 +2026,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="20">
         <v>12</v>
       </c>
@@ -2095,7 +2035,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -2104,7 +2044,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="20">
         <v>14</v>
       </c>
@@ -2113,7 +2053,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -2124,24 +2064,27 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -2150,28 +2093,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:5" ht="21">
+      <c r="B1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="29"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2180,11 +2123,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2193,11 +2136,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2206,11 +2149,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -2227,7 +2170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -2242,7 +2185,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="45">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -2257,7 +2200,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -2272,7 +2215,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -2287,7 +2230,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -2302,7 +2245,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -2311,7 +2254,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2320,7 +2263,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -2329,7 +2272,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -2338,7 +2281,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -2347,7 +2290,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="20">
         <v>11</v>
       </c>
@@ -2356,7 +2299,7 @@
       <c r="D18" s="19"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>12</v>
       </c>
@@ -2365,7 +2308,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="20">
         <v>13</v>
       </c>
@@ -2374,7 +2317,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>14</v>
       </c>
@@ -2383,7 +2326,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="20">
         <v>15</v>
       </c>
@@ -2394,24 +2337,27 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -2420,28 +2366,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:5" ht="21">
+      <c r="B1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="29"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2450,11 +2396,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2463,11 +2409,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2476,11 +2422,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -2497,7 +2443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="60">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -2512,7 +2458,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="75">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -2527,7 +2473,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="33" customHeight="1">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -2542,7 +2488,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -2557,7 +2503,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="60">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -2572,7 +2518,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -2581,7 +2527,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="12" customHeight="1">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2590,7 +2536,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="12" customHeight="1">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -2599,7 +2545,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -2608,7 +2554,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -2617,7 +2563,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -2626,7 +2572,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="20">
         <v>12</v>
       </c>
@@ -2635,7 +2581,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -2644,7 +2590,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="20">
         <v>14</v>
       </c>
@@ -2653,7 +2599,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -2664,24 +2610,27 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -2690,28 +2639,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:5" ht="21">
+      <c r="B1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="29"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2720,11 +2669,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2733,11 +2682,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2746,11 +2695,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -2767,7 +2716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -2782,7 +2731,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="30">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -2797,7 +2746,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -2812,7 +2761,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -2827,7 +2776,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -2842,7 +2791,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -2851,7 +2800,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="12" customHeight="1">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2860,7 +2809,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="12" customHeight="1">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -2869,7 +2818,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -2878,7 +2827,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -2887,7 +2836,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -2896,7 +2845,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="20">
         <v>12</v>
       </c>
@@ -2905,7 +2854,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -2914,7 +2863,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="20">
         <v>14</v>
       </c>
@@ -2923,7 +2872,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -2934,24 +2883,27 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -2960,28 +2912,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:5" ht="21">
+      <c r="B1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="29"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2990,11 +2942,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -3003,11 +2955,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -3016,11 +2968,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -3037,7 +2989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -3052,7 +3004,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="60">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -3067,7 +3019,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -3082,7 +3034,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -3097,7 +3049,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -3112,7 +3064,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -3121,7 +3073,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="12" customHeight="1">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -3130,7 +3082,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="12" customHeight="1">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -3139,7 +3091,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -3148,7 +3100,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -3157,7 +3109,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -3166,7 +3118,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="20">
         <v>12</v>
       </c>
@@ -3175,7 +3127,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -3184,7 +3136,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="20">
         <v>14</v>
       </c>
@@ -3193,7 +3145,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -3204,13 +3156,864 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21">
+      <c r="B1" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="E2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14">
+        <f>COUNTIF(D9:D100,"PASSED")</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <f>COUNTIF(D9:D100,"FAILED")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="16">
+        <f>SUM(D3:D4)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
+      <c r="A7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="11">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="30">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>5</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="30">
+      <c r="A20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="1">
+        <v>3</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="A24" s="1">
+        <v>4</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="1">
+        <v>5</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="1">
+        <v>6</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" ht="30">
+      <c r="A27" s="1">
+        <v>7</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="1">
+        <v>8</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="1">
+        <v>9</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="1">
+        <v>10</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="30">
+      <c r="A31" s="1">
+        <v>11</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="30">
+      <c r="A32" s="1">
+        <v>12</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="30">
+      <c r="A33" s="1">
+        <v>13</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" ht="30">
+      <c r="A34" s="1">
+        <v>14</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" ht="30">
+      <c r="A35" s="1">
+        <v>15</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" ht="30">
+      <c r="A36" s="1">
+        <v>16</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" ht="30">
+      <c r="A37" s="1">
+        <v>17</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" ht="30">
+      <c r="A38" s="1">
+        <v>18</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" ht="30">
+      <c r="A39" s="1">
+        <v>19</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" ht="30">
+      <c r="A40" s="1">
+        <v>20</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" ht="30">
+      <c r="A41" s="1">
+        <v>21</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" ht="30">
+      <c r="A42" s="1">
+        <v>22</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" ht="30">
+      <c r="A43" s="1">
+        <v>23</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" ht="30">
+      <c r="A44" s="1">
+        <v>24</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" ht="30">
+      <c r="A45" s="1">
+        <v>25</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" ht="45">
+      <c r="A47" s="1">
+        <v>26</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="11">
+        <v>27</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="11"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="1"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="1"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test cases for SET/Where clause
</commit_message>
<xml_diff>
--- a/testdb/updatetestcases/UpdateTestingDocument.xlsx
+++ b/testdb/updatetestcases/UpdateTestingDocument.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitscm\CS227Database\testdb\updatetestcases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
   </bookViews>
@@ -13,14 +18,14 @@
     <sheet name="Payment" sheetId="6" r:id="rId4"/>
     <sheet name="Product" sheetId="3" r:id="rId5"/>
     <sheet name="Si" sheetId="4" r:id="rId6"/>
-    <sheet name=" Intial Testing for CheckUpdate" sheetId="1" r:id="rId7"/>
+    <sheet name=" Intial Component Testing " sheetId="1" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="180">
   <si>
     <t>Test Condition</t>
   </si>
@@ -587,12 +592,6 @@
     <t>Check UPDATE spelling</t>
   </si>
   <si>
-    <t>Check missing SET</t>
-  </si>
-  <si>
-    <t>Check missing WHERE clause</t>
-  </si>
-  <si>
     <t>Syntax error in input</t>
   </si>
   <si>
@@ -678,13 +677,34 @@
   </si>
   <si>
     <t>update delivery set cost = '25000' where si_id = '10101' ;</t>
+  </si>
+  <si>
+    <t>update customer set last_name = 'roman' where first_name = 'ray</t>
+  </si>
+  <si>
+    <t>Check missing ' and ;</t>
+  </si>
+  <si>
+    <t>Check missing SET and wide spaces</t>
+  </si>
+  <si>
+    <t>update customer set last_name =                  'roman' where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>Query OK, 17 Row(s) affected                                                                        Row(s) matched: 17 Changed: 17</t>
+  </si>
+  <si>
+    <t>update customer set last_name = 'roman' where first_name =                        'ray' ;</t>
+  </si>
+  <si>
+    <t>Check missing WHERE clause and wide spaces</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -736,6 +756,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -784,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -853,8 +886,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -868,6 +911,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1126,19 +1177,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -1147,67 +1200,67 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="29" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="33"/>
       <c r="E2" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D8:D100,"PASSED")</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="28" t="s">
+        <f>COUNTIF(D8:D103,"PASSED")</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D8:D100,"FAILED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="29" t="s">
+        <f>COUNTIF(D8:D103,"FAILED")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D5" s="16">
         <f>SUM(D3:D4)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -1224,7 +1277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1235,7 +1288,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1">
+    <row r="9" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>1</v>
       </c>
@@ -1243,550 +1296,597 @@
         <v>54</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="17"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="28">
+        <v>2</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>5</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2" t="s">
+      <c r="C26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>3</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>4</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>5</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>6</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>7</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="30">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="45">
-      <c r="A17" s="1">
-        <v>2</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="30">
-      <c r="A18" s="1">
-        <v>3</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="30">
-      <c r="A19" s="1">
-        <v>4</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="45">
-      <c r="A20" s="1">
-        <v>5</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="30">
-      <c r="A22" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="30">
-      <c r="A23" s="1">
-        <v>1</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B33" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>9</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" ht="30">
-      <c r="A24" s="1">
-        <v>2</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B34" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>10</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="30">
-      <c r="A25" s="1">
-        <v>3</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="B35" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>11</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" ht="30">
-      <c r="A26" s="1">
-        <v>4</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B36" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>12</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" ht="30">
-      <c r="A27" s="1">
-        <v>5</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="B37" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>13</v>
       </c>
-      <c r="D27" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" ht="30">
-      <c r="A28" s="1">
-        <v>6</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B38" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>14</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" ht="30">
-      <c r="A29" s="1">
-        <v>7</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="B39" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>15</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" ht="30">
-      <c r="A30" s="1">
-        <v>8</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="B40" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>16</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" ht="30">
-      <c r="A31" s="1">
-        <v>9</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B41" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>17</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" ht="30">
-      <c r="A32" s="1">
-        <v>10</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="B42" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>18</v>
       </c>
-      <c r="D32" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" ht="30">
-      <c r="A33" s="1">
-        <v>11</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" s="10" t="s">
+      <c r="B43" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>19</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" ht="30">
-      <c r="A34" s="1">
-        <v>12</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C34" s="10" t="s">
+      <c r="B44" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>20</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" ht="30">
-      <c r="A35" s="1">
-        <v>13</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C35" s="10" t="s">
+      <c r="B45" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>21</v>
       </c>
-      <c r="D35" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" ht="30">
-      <c r="A36" s="1">
-        <v>14</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C36" s="10" t="s">
+      <c r="B46" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>22</v>
       </c>
-      <c r="D36" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" ht="30">
-      <c r="A37" s="1">
-        <v>15</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="C37" s="10" t="s">
+      <c r="B47" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>23</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:5" ht="30">
-      <c r="A38" s="1">
-        <v>16</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="B48" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>24</v>
       </c>
-      <c r="D38" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:5" ht="30">
-      <c r="A39" s="1">
-        <v>17</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="B49" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>25</v>
       </c>
-      <c r="D39" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" ht="30">
-      <c r="A40" s="1">
-        <v>18</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" ht="30">
-      <c r="A41" s="1">
-        <v>19</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:5" ht="30">
-      <c r="A42" s="1">
-        <v>20</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:5" ht="30">
-      <c r="A43" s="1">
-        <v>21</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="1:5" ht="30">
-      <c r="A44" s="1">
-        <v>22</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5" ht="30">
-      <c r="A45" s="1">
-        <v>23</v>
-      </c>
-      <c r="B45" s="6" t="s">
+      <c r="B50" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:5" ht="30">
-      <c r="A46" s="1">
-        <v>24</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5" ht="30">
-      <c r="A47" s="1">
-        <v>25</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C47" s="6" t="s">
+      <c r="C50" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D47" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="6"/>
+      <c r="D50" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1804,14 +1904,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -1820,28 +1920,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="29" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="33"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1850,11 +1950,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1863,11 +1963,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -1876,11 +1976,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -1897,7 +1997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -1912,7 +2012,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="45">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -1927,7 +2027,7 @@
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:5" ht="45">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -1942,7 +2042,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="60">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -1957,7 +2057,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="45">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -1972,7 +2072,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -1981,7 +2081,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1">
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -1990,7 +2090,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1">
+    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -1999,7 +2099,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -2008,7 +2108,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -2017,7 +2117,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -2026,7 +2126,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>12</v>
       </c>
@@ -2035,7 +2135,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -2044,7 +2144,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>14</v>
       </c>
@@ -2053,7 +2153,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -2077,14 +2177,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -2093,28 +2193,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="29" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="33"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2123,11 +2223,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2136,11 +2236,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2149,11 +2249,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -2170,7 +2270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -2185,7 +2285,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="45">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -2200,7 +2300,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="45">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -2215,7 +2315,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -2230,7 +2330,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -2245,7 +2345,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -2254,7 +2354,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2263,7 +2363,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -2272,7 +2372,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -2281,7 +2381,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -2290,7 +2390,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>11</v>
       </c>
@@ -2299,7 +2399,7 @@
       <c r="D18" s="19"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>12</v>
       </c>
@@ -2308,7 +2408,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>13</v>
       </c>
@@ -2317,7 +2417,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>14</v>
       </c>
@@ -2326,7 +2426,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>15</v>
       </c>
@@ -2350,14 +2450,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -2366,28 +2466,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="29" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="33"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2396,11 +2496,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2409,11 +2509,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2422,11 +2522,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -2443,7 +2543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -2458,7 +2558,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="75">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -2473,7 +2573,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="33" customHeight="1">
+    <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -2488,7 +2588,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -2503,7 +2603,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="60">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -2518,7 +2618,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -2527,7 +2627,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1">
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2536,7 +2636,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1">
+    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -2545,7 +2645,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -2554,7 +2654,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -2563,7 +2663,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -2572,7 +2672,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>12</v>
       </c>
@@ -2581,7 +2681,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -2590,7 +2690,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>14</v>
       </c>
@@ -2599,7 +2699,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -2623,14 +2723,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -2639,28 +2739,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="29" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="33"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2669,11 +2769,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2682,11 +2782,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2695,11 +2795,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -2716,7 +2816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -2731,7 +2831,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -2746,7 +2846,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="45">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -2761,7 +2861,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -2776,7 +2876,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -2791,7 +2891,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -2800,7 +2900,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1">
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2809,7 +2909,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1">
+    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -2818,7 +2918,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -2827,7 +2927,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -2836,7 +2936,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -2845,7 +2945,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>12</v>
       </c>
@@ -2854,7 +2954,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -2863,7 +2963,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>14</v>
       </c>
@@ -2872,7 +2972,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -2896,14 +2996,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -2912,28 +3012,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="29" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="33"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2942,11 +3042,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2955,11 +3055,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2968,11 +3068,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -2989,7 +3089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -3004,7 +3104,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="60">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>2</v>
       </c>
@@ -3019,7 +3119,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -3034,7 +3134,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -3049,7 +3149,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -3064,7 +3164,7 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -3073,7 +3173,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1">
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -3082,7 +3182,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1">
+    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -3091,7 +3191,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -3100,7 +3200,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -3109,7 +3209,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -3118,7 +3218,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>12</v>
       </c>
@@ -3127,7 +3227,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -3136,7 +3236,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>14</v>
       </c>
@@ -3145,7 +3245,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -3169,14 +3269,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
@@ -3185,28 +3285,28 @@
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="29" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="33"/>
       <c r="E2" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -3215,11 +3315,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -3228,11 +3328,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -3241,11 +3341,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>52</v>
       </c>
@@ -3262,7 +3362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -3273,7 +3373,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>1</v>
       </c>
@@ -3290,7 +3390,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -3301,7 +3401,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -3316,14 +3416,14 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="19"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -3334,7 +3434,7 @@
       <c r="D13" s="17"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -3349,7 +3449,7 @@
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -3364,7 +3464,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -3379,7 +3479,7 @@
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -3394,7 +3494,7 @@
       </c>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -3409,14 +3509,14 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="19"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="30">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>130</v>
       </c>
@@ -3427,7 +3527,7 @@
       <c r="D20" s="17"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -3442,7 +3542,7 @@
       </c>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="30">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -3457,7 +3557,7 @@
       </c>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -3472,7 +3572,7 @@
       </c>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -3487,7 +3587,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="30">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -3502,7 +3602,7 @@
       </c>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" ht="30">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -3517,7 +3617,7 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" ht="30">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>7</v>
       </c>
@@ -3532,7 +3632,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="30">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -3547,7 +3647,7 @@
       </c>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" ht="30">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>9</v>
       </c>
@@ -3562,7 +3662,7 @@
       </c>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>10</v>
       </c>
@@ -3577,7 +3677,7 @@
       </c>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>11</v>
       </c>
@@ -3592,7 +3692,7 @@
       </c>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>12</v>
       </c>
@@ -3607,7 +3707,7 @@
       </c>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="30">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>13</v>
       </c>
@@ -3622,7 +3722,7 @@
       </c>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="30">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>14</v>
       </c>
@@ -3637,7 +3737,7 @@
       </c>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>15</v>
       </c>
@@ -3652,7 +3752,7 @@
       </c>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>16</v>
       </c>
@@ -3667,7 +3767,7 @@
       </c>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="30">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>17</v>
       </c>
@@ -3682,7 +3782,7 @@
       </c>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="30">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>18</v>
       </c>
@@ -3697,7 +3797,7 @@
       </c>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="30">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>19</v>
       </c>
@@ -3712,7 +3812,7 @@
       </c>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="30">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>20</v>
       </c>
@@ -3727,7 +3827,7 @@
       </c>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>21</v>
       </c>
@@ -3742,7 +3842,7 @@
       </c>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="30">
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>22</v>
       </c>
@@ -3757,7 +3857,7 @@
       </c>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="30">
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>23</v>
       </c>
@@ -3772,7 +3872,7 @@
       </c>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="30">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>24</v>
       </c>
@@ -3787,7 +3887,7 @@
       </c>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="30">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>25</v>
       </c>
@@ -3802,14 +3902,14 @@
       </c>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="19"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="45">
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>26</v>
       </c>
@@ -3826,14 +3926,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="19"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>27</v>
       </c>
@@ -3850,154 +3950,154 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="19"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="19"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="19"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="19"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="19"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="19"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="19"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="19"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="19"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="19"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="19"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="19"/>
       <c r="E61" s="6"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="19"/>
       <c r="E62" s="6"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="19"/>
       <c r="E63" s="6"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="19"/>
       <c r="E64" s="6"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="19"/>
       <c r="E65" s="6"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="19"/>
       <c r="E66" s="6"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="19"/>
       <c r="E67" s="6"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="19"/>
       <c r="E68" s="6"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="19"/>
       <c r="E69" s="6"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="19"/>
       <c r="E70" s="6"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>

</xml_diff>

<commit_message>
add syntax and check table/column names test cases
</commit_message>
<xml_diff>
--- a/testdb/updatetestcases/UpdateTestingDocument.xlsx
+++ b/testdb/updatetestcases/UpdateTestingDocument.xlsx
@@ -5,27 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitscm\CS227Database\testdb\updatetestcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitscm\updatetestcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Check SET_WHERE" sheetId="7" r:id="rId1"/>
-    <sheet name="Customer" sheetId="2" r:id="rId2"/>
-    <sheet name="Delivery" sheetId="5" r:id="rId3"/>
-    <sheet name="Payment" sheetId="6" r:id="rId4"/>
-    <sheet name="Product" sheetId="3" r:id="rId5"/>
-    <sheet name="Si" sheetId="4" r:id="rId6"/>
-    <sheet name=" Intial Component Testing " sheetId="1" r:id="rId7"/>
+    <sheet name="SYNTAX" sheetId="8" r:id="rId1"/>
+    <sheet name="Check Tables_ColumnNames" sheetId="7" r:id="rId2"/>
+    <sheet name="Customer" sheetId="2" r:id="rId3"/>
+    <sheet name="Delivery" sheetId="5" r:id="rId4"/>
+    <sheet name="Payment" sheetId="6" r:id="rId5"/>
+    <sheet name="Product" sheetId="3" r:id="rId6"/>
+    <sheet name="Si" sheetId="4" r:id="rId7"/>
+    <sheet name=" Intial Component Testing " sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="230">
   <si>
     <t>Test Condition</t>
   </si>
@@ -574,9 +575,6 @@
     <t>Check table existing/spelling with set/where clause</t>
   </si>
   <si>
-    <t>Check column names existing/spelling in each table with set/where clause</t>
-  </si>
-  <si>
     <t>update prodct set description = 'technology' WHERE stock &lt; '87' AND stock &gt; '80' ;</t>
   </si>
   <si>
@@ -595,116 +593,313 @@
     <t>Syntax error in input</t>
   </si>
   <si>
+    <t>update customer l_name = 'roman' where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>update customers set l_name = 'roman' where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>update customer set lname = 'roman' where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>update customer set fname = 'ray' where last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>update customer set emails = 'a@gov.com' where last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>update customer set bdate = '7/7/1999' where last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>update customer set cust_id = '8'  where last_name = 'roman' ;</t>
+  </si>
+  <si>
+    <t>update payment set pay_id = '100' where amount = '5000' ;</t>
+  </si>
+  <si>
+    <t>update payment set sid = '500' where amount = '5000' ;</t>
+  </si>
+  <si>
+    <t>update payment set amt = '5000'  where payment_id = '100' ;</t>
+  </si>
+  <si>
+    <t>update payment set paymentdate = '5/5/2015' where payment_id = '100' ;</t>
+  </si>
+  <si>
+    <t>update payment set paymentmode = 'credit card' where payment_id = '100' ;</t>
+  </si>
+  <si>
+    <t>update si set sid = '1000' where price = '1500' ;</t>
+  </si>
+  <si>
+    <t>update si set cust_id = '1000' where price = '1500' ;</t>
+  </si>
+  <si>
+    <t>update si set prod_id = '1000' where price = '1500' ;</t>
+  </si>
+  <si>
+    <t>update si set dateorder = '10/10/10' where price = '1500' ;</t>
+  </si>
+  <si>
+    <t>update si set prices = '1500' where si_id = '1000' ;</t>
+  </si>
+  <si>
+    <t>update product set p_id = '10' where weight = '350' ;</t>
+  </si>
+  <si>
+    <t>update product set product_model = 'g9xafnhmex' where weight = '350' ;</t>
+  </si>
+  <si>
+    <t>update product set p_stock = '10' where weight = '350' ;</t>
+  </si>
+  <si>
+    <t>update product set p_desc = 'technology' where weight = '350' ;</t>
+  </si>
+  <si>
+    <t>update product set p_weight = '350' where model = '1960s' ;</t>
+  </si>
+  <si>
+    <t>update delivery set d_id = '11111' where delivery_cost = '25000' ;</t>
+  </si>
+  <si>
+    <t>update delivery set sid = '10101' where delivery_cost = '25000' ;</t>
+  </si>
+  <si>
+    <t>update delivery set qty = '15' where delivery_cost = '25000' ;</t>
+  </si>
+  <si>
+    <t>update delivery set date = '11/11/2015' where delivery_cost = '25000' ;</t>
+  </si>
+  <si>
+    <t>update delivery set cost = '25000' where si_id = '10101' ;</t>
+  </si>
+  <si>
+    <t>update customer set last_name = 'roman' where first_name = 'ray</t>
+  </si>
+  <si>
+    <t>Check missing ' and ;</t>
+  </si>
+  <si>
+    <t>update customer set last_name =                  'roman' where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>Query OK, 17 Row(s) affected                                                                        Row(s) matched: 17 Changed: 17</t>
+  </si>
+  <si>
+    <t>update customer set last_name = 'roman' where first_name =                        'ray' ;</t>
+  </si>
+  <si>
+    <t>update customer set last_name 'roman' where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>Check missing SET, wide spaces and syntax</t>
+  </si>
+  <si>
+    <t>Check missing WHERE clause, wide spaces and syntax</t>
+  </si>
+  <si>
+    <t>update customer set last_name =  'roman' were first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>update customer set last_name =  'roman' where first_name 'ray' ;</t>
+  </si>
+  <si>
+    <t>update customer set last_name =  'roman' where first_name = ray ;</t>
+  </si>
+  <si>
+    <t>wrong spelling update</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">update customer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> last_name =  'roman' where first_name = 'ray' ;</t>
+    </r>
+  </si>
+  <si>
+    <t>missing '='</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">update customer set last_name  = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>roman</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> where first_name = 'ray' ;</t>
+    </r>
+  </si>
+  <si>
+    <t>missing 'where'</t>
+  </si>
+  <si>
+    <t>misspelled 'where'</t>
+  </si>
+  <si>
+    <t>missing 'set'</t>
+  </si>
+  <si>
+    <t>misspelled 'set'</t>
+  </si>
+  <si>
+    <t>missing ' ' for string ('roman')</t>
+  </si>
+  <si>
+    <t>missing ' ' for string ('ray')</t>
+  </si>
+  <si>
+    <t>update customer set last_name = 'roman' where first_name = 'ray'</t>
+  </si>
+  <si>
+    <t>Check missing ' ;'</t>
+  </si>
+  <si>
+    <t>'last_name'</t>
+  </si>
+  <si>
+    <t>'first_name'</t>
+  </si>
+  <si>
+    <t>'email'</t>
+  </si>
+  <si>
+    <t>'date_ordered'</t>
+  </si>
+  <si>
+    <t>'price'</t>
+  </si>
+  <si>
+    <t>'product_id'</t>
+  </si>
+  <si>
+    <t>'model'</t>
+  </si>
+  <si>
+    <t>'stock'</t>
+  </si>
+  <si>
+    <t>'description'</t>
+  </si>
+  <si>
+    <t>'weight'</t>
+  </si>
+  <si>
+    <t>'delivery_id'</t>
+  </si>
+  <si>
+    <t>'si_id'</t>
+  </si>
+  <si>
+    <t>'quantity'</t>
+  </si>
+  <si>
+    <t>'delivery_date'</t>
+  </si>
+  <si>
+    <t>'delivery_cost'</t>
+  </si>
+  <si>
+    <t>'customer'</t>
+  </si>
+  <si>
+    <t>'product'</t>
+  </si>
+  <si>
+    <t>'si'</t>
+  </si>
+  <si>
+    <t>'delivery'</t>
+  </si>
+  <si>
+    <t>'payment'</t>
+  </si>
+  <si>
+    <t>'birthdate'</t>
+  </si>
+  <si>
+    <t>'customer_id'</t>
+  </si>
+  <si>
+    <t>'payment_id'</t>
+  </si>
+  <si>
+    <t>'amount'</t>
+  </si>
+  <si>
+    <t>'date_of_payment'</t>
+  </si>
+  <si>
+    <t>'mode_of_payment'</t>
+  </si>
+  <si>
+    <t>Check column names existing/spelling with set/where clause in table 'payment'</t>
+  </si>
+  <si>
+    <t>Check column names existing/spelling with set/where clause in table 'customer'</t>
+  </si>
+  <si>
+    <t>Check column names existing/spelling with set/where clause in table 'si'</t>
+  </si>
+  <si>
+    <t>Check column names existing/spelling with set/where clause in table 'product'</t>
+  </si>
+  <si>
+    <t>Check column names existing/spelling with set/where clause in table 'delivery'</t>
+  </si>
+  <si>
     <t>E</t>
   </si>
   <si>
-    <t>update customer l_name = 'roman' where first_name = 'ray' ;</t>
-  </si>
-  <si>
-    <t>update customers set l_name = 'roman' where first_name = 'ray' ;</t>
-  </si>
-  <si>
-    <t>update customer set lname = 'roman' where first_name = 'ray' ;</t>
-  </si>
-  <si>
-    <t>update customer set fname = 'ray' where last_name = 'roman' ;</t>
-  </si>
-  <si>
-    <t>update customer set emails = 'a@gov.com' where last_name = 'roman' ;</t>
-  </si>
-  <si>
-    <t>update customer set bdate = '7/7/1999' where last_name = 'roman' ;</t>
-  </si>
-  <si>
-    <t>update customer set cust_id = '8'  where last_name = 'roman' ;</t>
-  </si>
-  <si>
-    <t>update payment set pay_id = '100' where amount = '5000' ;</t>
-  </si>
-  <si>
-    <t>update payment set sid = '500' where amount = '5000' ;</t>
-  </si>
-  <si>
-    <t>update payment set amt = '5000'  where payment_id = '100' ;</t>
-  </si>
-  <si>
-    <t>update payment set paymentdate = '5/5/2015' where payment_id = '100' ;</t>
-  </si>
-  <si>
-    <t>update payment set paymentmode = 'credit card' where payment_id = '100' ;</t>
-  </si>
-  <si>
-    <t>update si set sid = '1000' where price = '1500' ;</t>
-  </si>
-  <si>
-    <t>update si set cust_id = '1000' where price = '1500' ;</t>
-  </si>
-  <si>
-    <t>update si set prod_id = '1000' where price = '1500' ;</t>
-  </si>
-  <si>
-    <t>update si set dateorder = '10/10/10' where price = '1500' ;</t>
-  </si>
-  <si>
-    <t>update si set prices = '1500' where si_id = '1000' ;</t>
-  </si>
-  <si>
-    <t>update product set p_id = '10' where weight = '350' ;</t>
-  </si>
-  <si>
-    <t>update product set product_model = 'g9xafnhmex' where weight = '350' ;</t>
-  </si>
-  <si>
-    <t>update product set p_stock = '10' where weight = '350' ;</t>
-  </si>
-  <si>
-    <t>update product set p_desc = 'technology' where weight = '350' ;</t>
-  </si>
-  <si>
-    <t>update product set p_weight = '350' where model = '1960s' ;</t>
-  </si>
-  <si>
-    <t>update delivery set d_id = '11111' where delivery_cost = '25000' ;</t>
-  </si>
-  <si>
-    <t>update delivery set sid = '10101' where delivery_cost = '25000' ;</t>
-  </si>
-  <si>
-    <t>update delivery set qty = '15' where delivery_cost = '25000' ;</t>
-  </si>
-  <si>
-    <t>update delivery set date = '11/11/2015' where delivery_cost = '25000' ;</t>
-  </si>
-  <si>
-    <t>update delivery set cost = '25000' where si_id = '10101' ;</t>
-  </si>
-  <si>
-    <t>update customer set last_name = 'roman' where first_name = 'ray</t>
-  </si>
-  <si>
-    <t>Check missing ' and ;</t>
-  </si>
-  <si>
-    <t>Check missing SET and wide spaces</t>
-  </si>
-  <si>
-    <t>update customer set last_name =                  'roman' where first_name = 'ray' ;</t>
-  </si>
-  <si>
-    <t>Query OK, 17 Row(s) affected                                                                        Row(s) matched: 17 Changed: 17</t>
-  </si>
-  <si>
-    <t>update customer set last_name = 'roman' where first_name =                        'ray' ;</t>
-  </si>
-  <si>
-    <t>Check missing WHERE clause and wide spaces</t>
+    <t>F</t>
+  </si>
+  <si>
+    <t>update customer set last_name = 'roman'                    where first_name = 'ray' ;</t>
+  </si>
+  <si>
+    <t>acceptable wide space</t>
+  </si>
+  <si>
+    <t>update customer set last_name = 'roman' where first_name = 'ray'                                 ;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -769,6 +964,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -817,7 +1018,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -899,11 +1100,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1185,9 +1391,441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="E2" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14">
+        <f>COUNTIF(D8:D84,"PASSED")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <f>COUNTIF(D8:D84,"FAILED")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="16">
+        <f>SUM(D3:D4)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>5</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>6</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="28">
+        <v>4</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="28">
+        <v>5</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="34">
+        <v>6</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="34">
+        <v>7</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>8</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -1201,59 +1839,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="36"/>
       <c r="E2" s="4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D8:D103,"PASSED")</f>
-        <v>35</v>
+        <f>COUNTIF(D8:D97,"PASSED")</f>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D8:D103,"FAILED")</f>
-        <v>1</v>
+        <f>COUNTIF(D8:D97,"FAILED")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D5" s="16">
         <f>SUM(D3:D4)</f>
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1277,616 +1915,588 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="17"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="5"/>
+      <c r="B9" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>144</v>
+        <v>139</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="37" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>177</v>
+        <v>140</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>4</v>
-      </c>
+      <c r="E12" s="37" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
-        <v>2</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>174</v>
-      </c>
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>3</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E19" s="37" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="37" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>3</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="6"/>
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E22" s="37" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="6"/>
+      <c r="E23" s="37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>3</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="5"/>
+      <c r="A25" s="1">
+        <v>4</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="37" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>2</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="6"/>
+      <c r="A27" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>11</v>
+        <v>156</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="37" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>12</v>
+        <v>157</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="37" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>13</v>
+        <v>158</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="37" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>14</v>
+        <v>159</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="37" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>15</v>
+        <v>160</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="6"/>
+      <c r="E32" s="37" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>8</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="6"/>
+      <c r="A33" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="37" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="37" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>19</v>
+        <v>163</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="6"/>
+      <c r="E36" s="37" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>20</v>
+        <v>164</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="6"/>
+      <c r="E37" s="37" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>21</v>
+        <v>165</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="37" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>14</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="6"/>
+      <c r="A39" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>23</v>
+        <v>166</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="6"/>
+      <c r="E40" s="37" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="6"/>
+      <c r="E41" s="37" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E42" s="6"/>
+      <c r="E42" s="37" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="37" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D44" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>20</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>21</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>22</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>23</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>24</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>25</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="6"/>
+      <c r="E44" s="37" t="s">
+        <v>208</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1903,13 +2513,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1921,53 +2529,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="36"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D8:D51,"PASSED")</f>
+        <f>COUNTIF(D8:D46,"PASSED")</f>
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D8:D53,"FAILED")</f>
+        <f>COUNTIF(D8:D48,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2116,324 +2724,6 @@
       <c r="C17" s="6"/>
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>11</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
-        <v>12</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>13</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
-        <v>14</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>15</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-  </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="32" style="4" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="E2" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="14">
-        <f>COUNTIF(D8:D51,"PASSED")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="15">
-        <f>COUNTIF(D8:D53,"FAILED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="16">
-        <f>SUM(D3:D4)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
-        <v>1</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
-        <v>2</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
-        <v>4</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>5</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
-        <v>6</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>7</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
-        <v>8</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>9</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>10</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
-        <v>11</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>12</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
-        <v>13</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>14</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
-        <v>15</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2451,11 +2741,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2467,53 +2755,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="36"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D8:D51,"PASSED")</f>
+        <f>COUNTIF(D8:D46,"PASSED")</f>
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D8:D53,"FAILED")</f>
+        <f>COUNTIF(D8:D48,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2543,77 +2831,77 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>2</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>91</v>
+      <c r="B9" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>101</v>
+      <c r="B10" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="9"/>
@@ -2627,7 +2915,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2636,7 +2924,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>8</v>
       </c>
@@ -2655,58 +2943,13 @@
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="1">
         <v>10</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>11</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
-        <v>12</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>13</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
-        <v>14</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>15</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2724,11 +2967,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2740,53 +2981,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="36"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D8:D51,"PASSED")</f>
+        <f>COUNTIF(D8:D46,"PASSED")</f>
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D8:D53,"FAILED")</f>
+        <f>COUNTIF(D8:D48,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -2816,75 +3057,75 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>2</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>98</v>
+      <c r="B10" s="26" t="s">
+        <v>101</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>4</v>
@@ -2935,51 +3176,6 @@
       <c r="C17" s="6"/>
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>11</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
-        <v>12</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>13</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
-        <v>14</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>15</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2997,11 +3193,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3013,53 +3207,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="36"/>
       <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D8:D51,"PASSED")</f>
+        <f>COUNTIF(D8:D46,"PASSED")</f>
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D8:D53,"FAILED")</f>
+        <f>COUNTIF(D8:D48,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -3094,55 +3288,55 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>2</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>94</v>
+      <c r="B9" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>4</v>
@@ -3154,10 +3348,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>4</v>
@@ -3208,51 +3402,6 @@
       <c r="C17" s="6"/>
       <c r="D17" s="19"/>
       <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>11</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
-        <v>12</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>13</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
-        <v>14</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>15</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3270,11 +3419,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3286,53 +3433,279 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="36"/>
+      <c r="E2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14">
+        <f>COUNTIF(D8:D46,"PASSED")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <f>COUNTIF(D8:D48,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="16">
+        <f>SUM(D3:D4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>2</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="36"/>
       <c r="E2" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="14">
-        <f>COUNTIF(D9:D100,"PASSED")</f>
+        <f>COUNTIF(D9:D81,"PASSED")</f>
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="15">
-        <f>COUNTIF(D9:D100,"FAILED")</f>
+        <f>COUNTIF(D9:D81,"FAILED")</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
@@ -3970,139 +4343,6 @@
       <c r="C52" s="6"/>
       <c r="D52" s="19"/>
       <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="6"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="6"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="6"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="6"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="6"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="6"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="6"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="6"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="6"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="6"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="6"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="6"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>